<commit_message>
28-11-2018: Commit con programa de secop y comentarios sobre r para corregir
</commit_message>
<xml_diff>
--- a/syncfusion_payc/syncfusion_payc/VISTA_DETALLE_ADJUNTOS_PERS/adjuntosfactura/Adjunto_11899.xlsx
+++ b/syncfusion_payc/syncfusion_payc/VISTA_DETALLE_ADJUNTOS_PERS/adjuntosfactura/Adjunto_11899.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117" count="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94" count="320">
   <si>
     <t>Periodo Facturación</t>
   </si>
@@ -140,15 +140,6 @@
     <t>TIPO NOVEDAD:INCAPACIDAD - FECHA INICIO:Oct  5 2018 12:00AM - FECHA FIN:Oct  6 2018 12:00AM</t>
   </si>
   <si>
-    <t>RESIDENTE DE INSTALACIONES</t>
-  </si>
-  <si>
-    <t>JAIRO HERNAN WILLS RIANO</t>
-  </si>
-  <si>
-    <t>nov. 01 2017</t>
-  </si>
-  <si>
     <t>RESIDENTE ADMINISTRATIVO</t>
   </si>
   <si>
@@ -215,81 +206,45 @@
     <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM</t>
   </si>
   <si>
-    <t>MAREYEY FIQUE MORENO</t>
-  </si>
-  <si>
-    <t>ene. 02 2018</t>
+    <t>RESIDENTE SOTANOS</t>
+  </si>
+  <si>
+    <t>DIEGO ANDRES CERINZA HUERTAS</t>
+  </si>
+  <si>
+    <t>ene. 08 2016</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  6 2018 12:00AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESIDENTE DE COMERCIO </t>
+  </si>
+  <si>
+    <t>JENNY CONSTANZA CONTENTO FUENTES</t>
+  </si>
+  <si>
+    <t>ago. 24 2017</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  5 2018 12:00AM</t>
+  </si>
+  <si>
+    <t>RESIDENTE TORRE 1</t>
+  </si>
+  <si>
+    <t>JOHAN GABRIEL QUIROGA RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>ago. 09 2016</t>
   </si>
   <si>
     <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM</t>
   </si>
   <si>
-    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM</t>
-  </si>
-  <si>
-    <t>RESIDENTE SOTANOS</t>
-  </si>
-  <si>
-    <t>DIEGO ANDRES CERINZA HUERTAS</t>
-  </si>
-  <si>
-    <t>ene. 08 2016</t>
-  </si>
-  <si>
-    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  6 2018 12:00AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESIDENTE DE COMERCIO </t>
-  </si>
-  <si>
-    <t>JENNY CONSTANZA CONTENTO FUENTES</t>
-  </si>
-  <si>
-    <t>ago. 24 2017</t>
-  </si>
-  <si>
-    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  5 2018 12:00AM</t>
-  </si>
-  <si>
-    <t>RESIDENTE URBANISMO</t>
-  </si>
-  <si>
-    <t>LEONARDO ALBERTO DUSSAN GARCIA</t>
-  </si>
-  <si>
-    <t>ene. 24 2017</t>
-  </si>
-  <si>
-    <t>RESIDENTE TORRE 1</t>
-  </si>
-  <si>
-    <t>JOHAN GABRIEL QUIROGA RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>ago. 09 2016</t>
-  </si>
-  <si>
     <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  8 2018 12:00AM</t>
   </si>
   <si>
-    <t>INSPECTOR SOTANOS</t>
-  </si>
-  <si>
-    <t>LUIS ORLANDO CARDOZO ZORRO</t>
-  </si>
-  <si>
-    <t>jun. 11 2017</t>
-  </si>
-  <si>
-    <t>TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  2 2018  2:30AM, TIPO NOVEDAD:HORAS_EXTRAS_NOCTURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  2:30AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  2 2018 12:00AM</t>
-  </si>
-  <si>
-    <t>TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep 10 2018 12:00AM</t>
-  </si>
-  <si>
-    <t>TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  1 2018  2:30PM</t>
-  </si>
-  <si>
     <t>INSPECTOR COMERCIO</t>
   </si>
   <si>
@@ -336,30 +291,6 @@
   </si>
   <si>
     <t>TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  2 2018  2:30AM</t>
-  </si>
-  <si>
-    <t>INSPECTOR TORRE 2</t>
-  </si>
-  <si>
-    <t>JORGE EDUARDO YAZO PATARROYO</t>
-  </si>
-  <si>
-    <t>oct. 12 2016</t>
-  </si>
-  <si>
-    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM</t>
-  </si>
-  <si>
-    <t>RESIDENTE AMBIENTAL</t>
-  </si>
-  <si>
-    <t>CLAUDIA MARCELA DIAZ BARBOSA</t>
-  </si>
-  <si>
-    <t>oct. 01 2018</t>
-  </si>
-  <si>
-    <t>TIPO NOVEDAD:INCAPACIDAD - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  2 2018 12:00AM</t>
   </si>
   <si>
     <t>PAMELA OCAMPO GRISALES</t>
@@ -675,9 +606,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:d1p1="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" d1p1:id="rId1" refreshedBy="DefaultAppPool" refreshedDate="43427.384906631945" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" refreshOnLoad="1" recordCount="0">
+<pivotCacheDefinition xmlns:d1p1="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" d1p1:id="rId1" refreshedBy="DefaultAppPool" refreshedDate="43430.674432002314" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" refreshOnLoad="1" recordCount="0">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A3:X56" sheet="BASE DE DATOS"/>
+    <worksheetSource ref="A3:X40" sheet="BASE DE DATOS"/>
   </cacheSource>
   <cacheFields count="24">
     <cacheField name="Periodo Facturación" numFmtId="0">
@@ -711,42 +642,31 @@
       <sharedItems>
         <s v="COORDINADOR"/>
         <s v="DIRECTOR"/>
-        <s v="RESIDENTE DE INSTALACIONES"/>
         <s v="RESIDENTE ADMINISTRATIVO"/>
         <s v="AUXILIAR ADMINISTRATIVO"/>
         <s v="RESIDENTE SOTANOS"/>
         <s v="RESIDENTE DE COMERCIO "/>
-        <s v="RESIDENTE URBANISMO"/>
         <s v="RESIDENTE TORRE 1"/>
-        <s v="INSPECTOR SOTANOS"/>
         <s v="INSPECTOR COMERCIO"/>
         <s v="INSPECTOR TORRE 1"/>
         <s v="INSPECTOR TORRE 1 ESTRUCTURA"/>
-        <s v="INSPECTOR TORRE 2"/>
-        <s v="RESIDENTE AMBIENTAL"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Nombre colaborador / Item" numFmtId="0">
       <sharedItems>
         <s v="CARLOS ALFREDO NEIRA GRAJALES"/>
         <s v="JORGE ENRIQUE CASSALETT BUSTILLO"/>
-        <s v="JAIRO HERNAN WILLS RIANO"/>
         <s v="MARIA PIEDAD ESPINOSA VIRGUEZ"/>
         <s v="LORNA ROCIO SANCHEZ ROLDAN"/>
         <s v="YEIMY KATERINE PIRAJAN APARICIO"/>
         <s v="RUBY TATIANA PERDIGON DE LOS RIOS"/>
         <s v="SEBASTIAN FELIPE DIAZ RIVEROS"/>
-        <s v="MAREYEY FIQUE MORENO"/>
         <s v="DIEGO ANDRES CERINZA HUERTAS"/>
         <s v="JENNY CONSTANZA CONTENTO FUENTES"/>
-        <s v="LEONARDO ALBERTO DUSSAN GARCIA"/>
         <s v="JOHAN GABRIEL QUIROGA RODRIGUEZ"/>
-        <s v="LUIS ORLANDO CARDOZO ZORRO"/>
         <s v="VICTOR MANUEL AVENDANO LEON"/>
         <s v="EBERTO LIBARDO BRAVO MENESES"/>
         <s v="PEDRO PABLO HERRERA SALDARRIAGA"/>
-        <s v="JORGE EDUARDO YAZO PATARROYO"/>
-        <s v="CLAUDIA MARCELA DIAZ BARBOSA"/>
         <s v="PAMELA OCAMPO GRISALES"/>
       </sharedItems>
     </cacheField>
@@ -754,23 +674,17 @@
       <sharedItems>
         <s v="may. 01 2018"/>
         <s v="sep. 01 2016"/>
-        <s v="nov. 01 2017"/>
         <s v="ago. 15 2016"/>
         <s v="sep. 26 2017"/>
         <s v="feb. 13 2017"/>
         <s v="oct. 25 2016"/>
         <s v="dic. 11 2016"/>
-        <s v="ene. 02 2018"/>
         <s v="ene. 08 2016"/>
         <s v="ago. 24 2017"/>
-        <s v="ene. 24 2017"/>
         <s v="ago. 09 2016"/>
-        <s v="jun. 11 2017"/>
         <s v="oct. 10 2017"/>
         <s v="ene. 14 2015"/>
         <s v="sep. 16 2015"/>
-        <s v="oct. 12 2016"/>
-        <s v="oct. 01 2018"/>
         <s v="oct. 20 2016"/>
       </sharedItems>
     </cacheField>
@@ -788,7 +702,6 @@
         <n v="9003523.9424"/>
         <n v="8643382.984704"/>
         <n v="10083946.815488"/>
-        <n v="9084536.64768"/>
         <n v="4820051.238912"/>
         <n v="4303617.1776"/>
         <n v="5164340.61312"/>
@@ -801,20 +714,12 @@
         <n v="2016602.185728"/>
         <n v="3558709.73952"/>
         <n v="3202838.765568"/>
-        <n v="3440086.081536"/>
-        <n v="3321462.423552"/>
         <n v="5971893.4576708"/>
         <n v="7464866.8220885"/>
         <n v="6220722.35174042"/>
-        <n v="6106661.6832"/>
-        <n v="5896087.1424"/>
-        <n v="6317236.224"/>
         <n v="7216038.555648"/>
         <n v="5474236.145664"/>
         <n v="7464867.47136"/>
-        <n v="3797207.341824"/>
-        <n v="2758965.18144"/>
-        <n v="3748199.40768"/>
         <n v="3602990.71392"/>
         <n v="2555673.010176"/>
         <n v="3639292.88736"/>
@@ -823,21 +728,15 @@
         <n v="3759090.059712"/>
         <n v="3877072.123392"/>
         <n v="3966012.44832"/>
-        <n v="3252674.740224"/>
-        <n v="3368841.695232"/>
-        <n v="3485008.65024"/>
-        <n v="6967209.09829149"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Salario básico" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="1853904"/>
         <n v="6403280"/>
-        <n v="5384080"/>
         <n v="3060720"/>
         <n v="2109120"/>
         <n v="4424159.6152"/>
-        <n v="3744000"/>
         <n v="4424160"/>
         <n v="2065440"/>
       </sharedItems>
@@ -852,15 +751,12 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="3378331.58787072"/>
         <n v="10804228.73088"/>
-        <n v="9084536.64768"/>
         <n v="5164340.61312"/>
         <n v="1205012.809728"/>
         <n v="3558709.73952"/>
         <n v="7464866.8220885"/>
-        <n v="6317236.224"/>
         <n v="7464867.47136"/>
         <n v="3485008.65024"/>
-        <n v="7464866.88643072"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Descuentos (Novedades)" numFmtId="0">
@@ -878,19 +774,12 @@
         <n v="-1067612.921856"/>
         <n v="-1542107.553792"/>
         <n v="-355870.973952"/>
-        <n v="-118623.657984"/>
-        <n v="-237247.315968"/>
         <n v="-1492973.3644177"/>
         <n v="-1244144.47034808"/>
-        <n v="-210574.5408"/>
-        <n v="-421149.0816"/>
         <n v="-248828.915712"/>
         <n v="-1990631.325696"/>
-        <n v="-232333.910016"/>
-        <n v="-1161669.55008"/>
         <n v="-929335.640064"/>
         <n v="-116166.955008"/>
-        <n v="-497657.788139233"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Total horas novedades" numFmtId="0">
@@ -905,7 +794,6 @@
         <n v="72"/>
         <n v="104"/>
         <n v="8"/>
-        <n v="80"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Total días novedades" numFmtId="0">
@@ -920,15 +808,11 @@
         <n v="9"/>
         <n v="13"/>
         <n v="1"/>
-        <n v="10"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Horas Extra" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="0"/>
-        <n v="544532.6016"/>
-        <n v="435626.08128"/>
-        <n v="263190.75744"/>
         <n v="117982.06368"/>
         <n v="154284.23712"/>
         <n v="99830.97696"/>
@@ -941,21 +825,18 @@
     <cacheField name="HE Diurnas" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="0"/>
-        <n v="26.5"/>
-        <n v="24"/>
-        <n v="14.5"/>
         <n v="6.5"/>
         <n v="8.5"/>
         <n v="5.5"/>
         <n v="6"/>
         <n v="21.5"/>
         <n v="28"/>
+        <n v="26.5"/>
       </sharedItems>
     </cacheField>
     <cacheField name="HE Nocturnas" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1">
         <n v="0"/>
-        <n v="2.5"/>
       </sharedItems>
     </cacheField>
     <cacheField name="HE Festivas Diurnas" numFmtId="0">
@@ -969,7 +850,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Detalle Novedades" numFmtId="0">
-      <sharedItems longText="1">
+      <sharedItems>
         <s v="SIN NOVEDADES ago. 2018"/>
         <s v="SIN NOVEDADES sep. 2018"/>
         <s v="SIN NOVEDADES oct. 2018"/>
@@ -984,14 +865,10 @@
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  9 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep 12 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM"/>
-        <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM"/>
-        <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  6 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  5 2018 12:00AM"/>
+        <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  8 2018 12:00AM"/>
-        <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  2 2018  2:30AM, TIPO NOVEDAD:HORAS_EXTRAS_NOCTURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  2:30AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  2 2018 12:00AM"/>
-        <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep 10 2018 12:00AM"/>
-        <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  1 2018  2:30PM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  6:30AM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  8:30AM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018  5:30AM"/>
@@ -999,8 +876,6 @@
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  9:30PM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018  4:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  2 2018  2:30AM"/>
-        <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM"/>
-        <s v="TIPO NOVEDAD:INCAPACIDAD - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  2 2018 12:00AM"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Dedicación" numFmtId="0">
@@ -1044,69 +919,52 @@
     </pivotField>
     <pivotField axis="axisRow" outline="0" compact="0" showAll="0" defaultSubtotal="0">
       <items>
-        <item x="4"/>
+        <item x="3"/>
         <item x="0"/>
         <item x="1"/>
-        <item x="10"/>
+        <item x="7"/>
+        <item x="8"/>
         <item x="9"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="3"/>
-        <item x="14"/>
-        <item x="6"/>
         <item x="2"/>
         <item x="5"/>
-        <item x="8"/>
-        <item x="7"/>
+        <item x="4"/>
+        <item x="6"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" outline="0" compact="0" showAll="0" defaultSubtotal="0">
       <items>
         <item x="0"/>
-        <item x="18"/>
+        <item x="7"/>
+        <item x="11"/>
+        <item x="8"/>
         <item x="9"/>
-        <item x="15"/>
+        <item x="1"/>
+        <item x="3"/>
         <item x="2"/>
+        <item x="13"/>
+        <item x="12"/>
+        <item x="5"/>
+        <item x="6"/>
         <item x="10"/>
-        <item x="12"/>
-        <item x="17"/>
-        <item x="1"/>
-        <item x="11"/>
         <item x="4"/>
-        <item x="13"/>
-        <item x="8"/>
-        <item x="3"/>
-        <item x="19"/>
-        <item x="16"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="14"/>
-        <item x="5"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" outline="0" compact="0" showAll="0" defaultSubtotal="0">
       <items>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="11"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="13"/>
+        <item x="5"/>
+        <item x="1"/>
         <item x="12"/>
         <item x="3"/>
-        <item x="10"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="15"/>
-        <item x="11"/>
-        <item x="5"/>
-        <item x="13"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="18"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="16"/>
-        <item x="4"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" outline="0" compact="0" showAll="0" defaultSubtotal="0">
@@ -1305,7 +1163,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="A1:X57"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -1900,25 +1758,25 @@
         <v>29</v>
       </c>
       <c r="J10" s="8">
-        <v>9084536.64768</v>
+        <v>4820051.238912</v>
       </c>
       <c r="K10" s="8">
-        <v>5384080</v>
+        <v>3060720</v>
       </c>
       <c r="L10" s="8">
         <v>0.5</v>
       </c>
       <c r="M10" s="8">
-        <v>9084536.64768</v>
+        <v>5164340.61312</v>
       </c>
       <c r="N10" s="8">
-        <v>0</v>
+        <v>-344289.374208</v>
       </c>
       <c r="O10" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P10" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="8">
         <v>0</v>
@@ -1936,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>31</v>
@@ -1972,25 +1830,25 @@
         <v>29</v>
       </c>
       <c r="J11" s="8">
-        <v>9084536.64768</v>
+        <v>4303617.1776</v>
       </c>
       <c r="K11" s="8">
-        <v>5384080</v>
+        <v>3060720</v>
       </c>
       <c r="L11" s="8">
         <v>0.5</v>
       </c>
       <c r="M11" s="8">
-        <v>9084536.64768</v>
+        <v>5164340.61312</v>
       </c>
       <c r="N11" s="8">
-        <v>0</v>
+        <v>-860723.43552</v>
       </c>
       <c r="O11" s="8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P11" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q11" s="8">
         <v>0</v>
@@ -2008,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>31</v>
@@ -2044,16 +1902,16 @@
         <v>29</v>
       </c>
       <c r="J12" s="8">
-        <v>9084536.64768</v>
+        <v>5164340.61312</v>
       </c>
       <c r="K12" s="8">
-        <v>5384080</v>
+        <v>3060720</v>
       </c>
       <c r="L12" s="8">
         <v>0.5</v>
       </c>
       <c r="M12" s="8">
-        <v>9084536.64768</v>
+        <v>5164340.61312</v>
       </c>
       <c r="N12" s="8">
         <v>0</v>
@@ -2104,19 +1962,19 @@
         <v>25</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="J13" s="8">
-        <v>4820051.238912</v>
+        <v>4647906.551808</v>
       </c>
       <c r="K13" s="8">
         <v>3060720</v>
@@ -2128,13 +1986,13 @@
         <v>5164340.61312</v>
       </c>
       <c r="N13" s="8">
-        <v>-344289.374208</v>
+        <v>-516434.061312</v>
       </c>
       <c r="O13" s="8">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="P13" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q13" s="8">
         <v>0</v>
@@ -2152,7 +2010,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>31</v>
@@ -2176,19 +2034,19 @@
         <v>25</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="J14" s="8">
-        <v>4303617.1776</v>
+        <v>4131472.490496</v>
       </c>
       <c r="K14" s="8">
         <v>3060720</v>
@@ -2200,13 +2058,13 @@
         <v>5164340.61312</v>
       </c>
       <c r="N14" s="8">
-        <v>-860723.43552</v>
+        <v>-1032868.122624</v>
       </c>
       <c r="O14" s="8">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="P14" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q14" s="8">
         <v>0</v>
@@ -2224,7 +2082,7 @@
         <v>0</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>31</v>
@@ -2248,19 +2106,19 @@
         <v>25</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="J15" s="8">
-        <v>5164340.61312</v>
+        <v>1205012.809728</v>
       </c>
       <c r="K15" s="8">
         <v>3060720</v>
@@ -2269,7 +2127,7 @@
         <v>0.5</v>
       </c>
       <c r="M15" s="8">
-        <v>5164340.61312</v>
+        <v>1205012.809728</v>
       </c>
       <c r="N15" s="8">
         <v>0</v>
@@ -2320,19 +2178,19 @@
         <v>25</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J16" s="8">
-        <v>4647906.551808</v>
+        <v>3787183.116288</v>
       </c>
       <c r="K16" s="8">
         <v>3060720</v>
@@ -2344,13 +2202,13 @@
         <v>5164340.61312</v>
       </c>
       <c r="N16" s="8">
-        <v>-516434.061312</v>
+        <v>-1377157.496832</v>
       </c>
       <c r="O16" s="8">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="P16" s="8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="Q16" s="8">
         <v>0</v>
@@ -2368,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W16" s="1" t="s">
         <v>31</v>
@@ -2392,19 +2250,19 @@
         <v>25</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J17" s="8">
-        <v>4131472.490496</v>
+        <v>3270749.054976</v>
       </c>
       <c r="K17" s="8">
         <v>3060720</v>
@@ -2416,13 +2274,13 @@
         <v>5164340.61312</v>
       </c>
       <c r="N17" s="8">
-        <v>-1032868.122624</v>
+        <v>-1893591.558144</v>
       </c>
       <c r="O17" s="8">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="P17" s="8">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q17" s="8">
         <v>0</v>
@@ -2440,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>31</v>
@@ -2451,7 +2309,7 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" s="7">
-        <v>43374</v>
+        <v>43313</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8">
@@ -2464,37 +2322,37 @@
         <v>25</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J18" s="8">
-        <v>1205012.809728</v>
+        <v>2491096.817664</v>
       </c>
       <c r="K18" s="8">
-        <v>3060720</v>
+        <v>2109120</v>
       </c>
       <c r="L18" s="8">
         <v>0.5</v>
       </c>
       <c r="M18" s="8">
-        <v>1205012.809728</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N18" s="8">
-        <v>0</v>
+        <v>-1067612.921856</v>
       </c>
       <c r="O18" s="8">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="P18" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q18" s="8">
         <v>0</v>
@@ -2512,18 +2370,18 @@
         <v>0</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X18" s="1">
-        <v>14236</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="7">
-        <v>43313</v>
+        <v>43344</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8">
@@ -2536,37 +2394,37 @@
         <v>25</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J19" s="8">
-        <v>3787183.116288</v>
+        <v>2016602.185728</v>
       </c>
       <c r="K19" s="8">
-        <v>3060720</v>
+        <v>2109120</v>
       </c>
       <c r="L19" s="8">
         <v>0.5</v>
       </c>
       <c r="M19" s="8">
-        <v>5164340.61312</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N19" s="8">
-        <v>-1377157.496832</v>
+        <v>-1542107.553792</v>
       </c>
       <c r="O19" s="8">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="P19" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="Q19" s="8">
         <v>0</v>
@@ -2584,18 +2442,18 @@
         <v>0</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="W19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X19" s="1">
-        <v>14291</v>
+        <v>14290</v>
       </c>
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="7">
-        <v>43344</v>
+        <v>43313</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8">
@@ -2608,37 +2466,37 @@
         <v>25</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="J20" s="8">
-        <v>3270749.054976</v>
+        <v>3558709.73952</v>
       </c>
       <c r="K20" s="8">
-        <v>3060720</v>
+        <v>2109120</v>
       </c>
       <c r="L20" s="8">
         <v>0.5</v>
       </c>
       <c r="M20" s="8">
-        <v>5164340.61312</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N20" s="8">
-        <v>-1893591.558144</v>
+        <v>0</v>
       </c>
       <c r="O20" s="8">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="P20" s="8">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="8">
         <v>0</v>
@@ -2656,18 +2514,18 @@
         <v>0</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X20" s="1">
-        <v>14290</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="21" spans="1:24">
       <c r="A21" s="7">
-        <v>43313</v>
+        <v>43344</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8">
@@ -2680,19 +2538,19 @@
         <v>25</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="J21" s="8">
-        <v>2491096.817664</v>
+        <v>3202838.765568</v>
       </c>
       <c r="K21" s="8">
         <v>2109120</v>
@@ -2704,13 +2562,13 @@
         <v>3558709.73952</v>
       </c>
       <c r="N21" s="8">
-        <v>-1067612.921856</v>
+        <v>-355870.973952</v>
       </c>
       <c r="O21" s="8">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="P21" s="8">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="Q21" s="8">
         <v>0</v>
@@ -2728,18 +2586,18 @@
         <v>0</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X21" s="1">
-        <v>14291</v>
+        <v>14290</v>
       </c>
     </row>
     <row r="22" spans="1:24">
       <c r="A22" s="7">
-        <v>43344</v>
+        <v>43374</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8">
@@ -2752,19 +2610,19 @@
         <v>25</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="J22" s="8">
-        <v>2016602.185728</v>
+        <v>3558709.73952</v>
       </c>
       <c r="K22" s="8">
         <v>2109120</v>
@@ -2776,13 +2634,13 @@
         <v>3558709.73952</v>
       </c>
       <c r="N22" s="8">
-        <v>-1542107.553792</v>
+        <v>0</v>
       </c>
       <c r="O22" s="8">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="P22" s="8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="8">
         <v>0</v>
@@ -2800,13 +2658,13 @@
         <v>0</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="W22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X22" s="1">
-        <v>14290</v>
+        <v>14236</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -2824,37 +2682,37 @@
         <v>25</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J23" s="8">
-        <v>3558709.73952</v>
+        <v>5971893.4576708</v>
       </c>
       <c r="K23" s="8">
-        <v>2109120</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L23" s="8">
         <v>0.5</v>
       </c>
       <c r="M23" s="8">
-        <v>3558709.73952</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N23" s="8">
-        <v>0</v>
+        <v>-1492973.3644177</v>
       </c>
       <c r="O23" s="8">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="P23" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q23" s="8">
         <v>0</v>
@@ -2872,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="W23" s="1" t="s">
         <v>31</v>
@@ -2896,37 +2754,37 @@
         <v>25</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J24" s="8">
-        <v>3202838.765568</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="K24" s="8">
-        <v>2109120</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L24" s="8">
         <v>0.5</v>
       </c>
       <c r="M24" s="8">
-        <v>3558709.73952</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N24" s="8">
-        <v>-355870.973952</v>
+        <v>0</v>
       </c>
       <c r="O24" s="8">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="P24" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="8">
         <v>0</v>
@@ -2944,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="W24" s="1" t="s">
         <v>31</v>
@@ -2968,28 +2826,28 @@
         <v>25</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J25" s="8">
-        <v>3558709.73952</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="K25" s="8">
-        <v>2109120</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L25" s="8">
         <v>0.5</v>
       </c>
       <c r="M25" s="8">
-        <v>3558709.73952</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N25" s="8">
         <v>0</v>
@@ -3040,37 +2898,37 @@
         <v>25</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J26" s="8">
-        <v>3440086.081536</v>
+        <v>6220722.35174042</v>
       </c>
       <c r="K26" s="8">
-        <v>2109120</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L26" s="8">
         <v>0.5</v>
       </c>
       <c r="M26" s="8">
-        <v>3558709.73952</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N26" s="8">
-        <v>-118623.657984</v>
+        <v>-1244144.47034808</v>
       </c>
       <c r="O26" s="8">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="P26" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q26" s="8">
         <v>0</v>
@@ -3088,7 +2946,7 @@
         <v>0</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="W26" s="1" t="s">
         <v>31</v>
@@ -3112,37 +2970,37 @@
         <v>25</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J27" s="8">
-        <v>3321462.423552</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="K27" s="8">
-        <v>2109120</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L27" s="8">
         <v>0.5</v>
       </c>
       <c r="M27" s="8">
-        <v>3558709.73952</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N27" s="8">
-        <v>-237247.315968</v>
+        <v>0</v>
       </c>
       <c r="O27" s="8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="P27" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="8">
         <v>0</v>
@@ -3160,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="W27" s="1" t="s">
         <v>31</v>
@@ -3184,28 +3042,28 @@
         <v>25</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J28" s="8">
-        <v>3558709.73952</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="K28" s="8">
-        <v>2109120</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L28" s="8">
         <v>0.5</v>
       </c>
       <c r="M28" s="8">
-        <v>3558709.73952</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N28" s="8">
         <v>0</v>
@@ -3256,37 +3114,37 @@
         <v>25</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J29" s="8">
-        <v>5971893.4576708</v>
+        <v>7216038.555648</v>
       </c>
       <c r="K29" s="8">
-        <v>4424159.6152</v>
+        <v>4424160</v>
       </c>
       <c r="L29" s="8">
         <v>0.5</v>
       </c>
       <c r="M29" s="8">
-        <v>7464866.8220885</v>
+        <v>7464867.47136</v>
       </c>
       <c r="N29" s="8">
-        <v>-1492973.3644177</v>
+        <v>-248828.915712</v>
       </c>
       <c r="O29" s="8">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="P29" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="8">
         <v>0</v>
@@ -3304,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W29" s="1" t="s">
         <v>31</v>
@@ -3328,37 +3186,37 @@
         <v>25</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J30" s="8">
-        <v>7464866.8220885</v>
+        <v>5474236.145664</v>
       </c>
       <c r="K30" s="8">
-        <v>4424159.6152</v>
+        <v>4424160</v>
       </c>
       <c r="L30" s="8">
         <v>0.5</v>
       </c>
       <c r="M30" s="8">
-        <v>7464866.8220885</v>
+        <v>7464867.47136</v>
       </c>
       <c r="N30" s="8">
-        <v>0</v>
+        <v>-1990631.325696</v>
       </c>
       <c r="O30" s="8">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="P30" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q30" s="8">
         <v>0</v>
@@ -3376,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="W30" s="1" t="s">
         <v>31</v>
@@ -3400,28 +3258,28 @@
         <v>25</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J31" s="8">
-        <v>7464866.8220885</v>
+        <v>7464867.47136</v>
       </c>
       <c r="K31" s="8">
-        <v>4424159.6152</v>
+        <v>4424160</v>
       </c>
       <c r="L31" s="8">
         <v>0.5</v>
       </c>
       <c r="M31" s="8">
-        <v>7464866.8220885</v>
+        <v>7464867.47136</v>
       </c>
       <c r="N31" s="8">
         <v>0</v>
@@ -3472,43 +3330,43 @@
         <v>25</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="J32" s="8">
-        <v>6220722.35174042</v>
+        <v>3602990.71392</v>
       </c>
       <c r="K32" s="8">
-        <v>4424159.6152</v>
+        <v>2065440</v>
       </c>
       <c r="L32" s="8">
         <v>0.5</v>
       </c>
       <c r="M32" s="8">
-        <v>7464866.8220885</v>
+        <v>3485008.65024</v>
       </c>
       <c r="N32" s="8">
-        <v>-1244144.47034808</v>
+        <v>0</v>
       </c>
       <c r="O32" s="8">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="P32" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="8">
-        <v>0</v>
+        <v>117982.06368</v>
       </c>
       <c r="R32" s="8">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="S32" s="8">
         <v>0</v>
@@ -3520,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="W32" s="1" t="s">
         <v>31</v>
@@ -3544,37 +3402,37 @@
         <v>25</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="J33" s="8">
-        <v>7464866.8220885</v>
+        <v>2555673.010176</v>
       </c>
       <c r="K33" s="8">
-        <v>4424159.6152</v>
+        <v>2065440</v>
       </c>
       <c r="L33" s="8">
         <v>0.5</v>
       </c>
       <c r="M33" s="8">
-        <v>7464866.8220885</v>
+        <v>3485008.65024</v>
       </c>
       <c r="N33" s="8">
-        <v>0</v>
+        <v>-929335.640064</v>
       </c>
       <c r="O33" s="8">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="P33" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q33" s="8">
         <v>0</v>
@@ -3592,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>31</v>
@@ -3603,7 +3461,7 @@
     </row>
     <row r="34" spans="1:24">
       <c r="A34" s="7">
-        <v>43374</v>
+        <v>43313</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8">
@@ -3616,28 +3474,28 @@
         <v>25</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J34" s="8">
-        <v>7464866.8220885</v>
+        <v>3639292.88736</v>
       </c>
       <c r="K34" s="8">
-        <v>4424159.6152</v>
+        <v>2065440</v>
       </c>
       <c r="L34" s="8">
         <v>0.5</v>
       </c>
       <c r="M34" s="8">
-        <v>7464866.8220885</v>
+        <v>3485008.65024</v>
       </c>
       <c r="N34" s="8">
         <v>0</v>
@@ -3649,10 +3507,10 @@
         <v>0</v>
       </c>
       <c r="Q34" s="8">
-        <v>0</v>
+        <v>154284.23712</v>
       </c>
       <c r="R34" s="8">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="S34" s="8">
         <v>0</v>
@@ -3664,18 +3522,18 @@
         <v>0</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X34" s="1">
-        <v>14236</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="35" spans="1:24">
       <c r="A35" s="7">
-        <v>43313</v>
+        <v>43344</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8">
@@ -3688,43 +3546,43 @@
         <v>25</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J35" s="8">
-        <v>6106661.6832</v>
+        <v>3584839.6272</v>
       </c>
       <c r="K35" s="8">
-        <v>3744000</v>
+        <v>2065440</v>
       </c>
       <c r="L35" s="8">
         <v>0.5</v>
       </c>
       <c r="M35" s="8">
-        <v>6317236.224</v>
+        <v>3485008.65024</v>
       </c>
       <c r="N35" s="8">
-        <v>-210574.5408</v>
+        <v>0</v>
       </c>
       <c r="O35" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P35" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="8">
-        <v>0</v>
+        <v>99830.97696</v>
       </c>
       <c r="R35" s="8">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="S35" s="8">
         <v>0</v>
@@ -3736,18 +3594,18 @@
         <v>0</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="W35" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X35" s="1">
-        <v>14291</v>
+        <v>14290</v>
       </c>
     </row>
     <row r="36" spans="1:24">
       <c r="A36" s="7">
-        <v>43344</v>
+        <v>43374</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8">
@@ -3760,43 +3618,43 @@
         <v>25</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J36" s="8">
-        <v>5896087.1424</v>
+        <v>3593915.17056</v>
       </c>
       <c r="K36" s="8">
-        <v>3744000</v>
+        <v>2065440</v>
       </c>
       <c r="L36" s="8">
         <v>0.5</v>
       </c>
       <c r="M36" s="8">
-        <v>6317236.224</v>
+        <v>3485008.65024</v>
       </c>
       <c r="N36" s="8">
-        <v>-421149.0816</v>
+        <v>0</v>
       </c>
       <c r="O36" s="8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="P36" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="8">
-        <v>0</v>
+        <v>108906.52032</v>
       </c>
       <c r="R36" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S36" s="8">
         <v>0</v>
@@ -3808,18 +3666,18 @@
         <v>0</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="W36" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X36" s="1">
-        <v>14290</v>
+        <v>14236</v>
       </c>
     </row>
     <row r="37" spans="1:24">
       <c r="A37" s="7">
-        <v>43374</v>
+        <v>43313</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8">
@@ -3832,43 +3690,43 @@
         <v>25</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J37" s="8">
-        <v>6317236.224</v>
+        <v>3759090.059712</v>
       </c>
       <c r="K37" s="8">
-        <v>3744000</v>
+        <v>2065440</v>
       </c>
       <c r="L37" s="8">
         <v>0.5</v>
       </c>
       <c r="M37" s="8">
-        <v>6317236.224</v>
+        <v>3485008.65024</v>
       </c>
       <c r="N37" s="8">
-        <v>0</v>
+        <v>-116166.955008</v>
       </c>
       <c r="O37" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P37" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q37" s="8">
-        <v>0</v>
+        <v>390248.36448</v>
       </c>
       <c r="R37" s="8">
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="S37" s="8">
         <v>0</v>
@@ -3880,18 +3738,18 @@
         <v>0</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="W37" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X37" s="1">
-        <v>14236</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="38" spans="1:24">
       <c r="A38" s="7">
-        <v>43313</v>
+        <v>43344</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8">
@@ -3904,31 +3762,31 @@
         <v>25</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J38" s="8">
-        <v>7216038.555648</v>
+        <v>3877072.123392</v>
       </c>
       <c r="K38" s="8">
-        <v>4424160</v>
+        <v>2065440</v>
       </c>
       <c r="L38" s="8">
         <v>0.5</v>
       </c>
       <c r="M38" s="8">
-        <v>7464867.47136</v>
+        <v>3485008.65024</v>
       </c>
       <c r="N38" s="8">
-        <v>-248828.915712</v>
+        <v>-116166.955008</v>
       </c>
       <c r="O38" s="8">
         <v>8</v>
@@ -3937,10 +3795,10 @@
         <v>1</v>
       </c>
       <c r="Q38" s="8">
-        <v>0</v>
+        <v>508230.42816</v>
       </c>
       <c r="R38" s="8">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="S38" s="8">
         <v>0</v>
@@ -3952,18 +3810,18 @@
         <v>0</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X38" s="1">
-        <v>14291</v>
+        <v>14290</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="A39" s="7">
-        <v>43344</v>
+        <v>43374</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8">
@@ -3976,43 +3834,43 @@
         <v>25</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J39" s="8">
-        <v>5474236.145664</v>
+        <v>3966012.44832</v>
       </c>
       <c r="K39" s="8">
-        <v>4424160</v>
+        <v>2065440</v>
       </c>
       <c r="L39" s="8">
         <v>0.5</v>
       </c>
       <c r="M39" s="8">
-        <v>7464867.47136</v>
+        <v>3485008.65024</v>
       </c>
       <c r="N39" s="8">
-        <v>-1990631.325696</v>
+        <v>0</v>
       </c>
       <c r="O39" s="8">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="P39" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="8">
-        <v>0</v>
+        <v>481003.79808</v>
       </c>
       <c r="R39" s="8">
-        <v>0</v>
+        <v>26.5</v>
       </c>
       <c r="S39" s="8">
         <v>0</v>
@@ -4024,18 +3882,18 @@
         <v>0</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X39" s="1">
-        <v>14290</v>
+        <v>14236</v>
       </c>
     </row>
     <row r="40" spans="1:24">
       <c r="A40" s="7">
-        <v>43374</v>
+        <v>43313</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8">
@@ -4048,16 +3906,16 @@
         <v>25</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="J40" s="8">
         <v>7464867.47136</v>
@@ -4096,1192 +3954,40 @@
         <v>0</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="W40" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X40" s="1">
-        <v>14236</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="41" spans="1:24">
-      <c r="A41" s="7">
-        <v>43313</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J41" s="8">
-        <v>3797207.341824</v>
-      </c>
-      <c r="K41" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L41" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M41" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N41" s="8">
-        <v>-232333.910016</v>
-      </c>
-      <c r="O41" s="8">
-        <v>16</v>
-      </c>
-      <c r="P41" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q41" s="8">
-        <v>544532.6016</v>
-      </c>
-      <c r="R41" s="8">
-        <v>26.5</v>
-      </c>
-      <c r="S41" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="T41" s="8">
-        <v>0</v>
-      </c>
-      <c r="U41" s="8">
-        <v>0</v>
-      </c>
-      <c r="V41" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="W41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X41" s="1">
-        <v>14291</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24">
-      <c r="A42" s="7">
-        <v>43344</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I42" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J42" s="8">
-        <v>2758965.18144</v>
-      </c>
-      <c r="K42" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L42" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M42" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N42" s="8">
-        <v>-1161669.55008</v>
-      </c>
-      <c r="O42" s="8">
-        <v>80</v>
-      </c>
-      <c r="P42" s="8">
-        <v>10</v>
-      </c>
-      <c r="Q42" s="8">
-        <v>435626.08128</v>
-      </c>
-      <c r="R42" s="8">
-        <v>24</v>
-      </c>
-      <c r="S42" s="8">
-        <v>0</v>
-      </c>
-      <c r="T42" s="8">
-        <v>0</v>
-      </c>
-      <c r="U42" s="8">
-        <v>0</v>
-      </c>
-      <c r="V42" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W42" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X42" s="1">
-        <v>14290</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24">
-      <c r="A43" s="7">
-        <v>43374</v>
-      </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I43" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J43" s="8">
-        <v>3748199.40768</v>
-      </c>
-      <c r="K43" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L43" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M43" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N43" s="8">
-        <v>0</v>
-      </c>
-      <c r="O43" s="8">
-        <v>0</v>
-      </c>
-      <c r="P43" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="8">
-        <v>263190.75744</v>
-      </c>
-      <c r="R43" s="8">
-        <v>14.5</v>
-      </c>
-      <c r="S43" s="8">
-        <v>0</v>
-      </c>
-      <c r="T43" s="8">
-        <v>0</v>
-      </c>
-      <c r="U43" s="8">
-        <v>0</v>
-      </c>
-      <c r="V43" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W43" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X43" s="1">
-        <v>14236</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24">
-      <c r="A44" s="7">
-        <v>43313</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J44" s="8">
-        <v>3602990.71392</v>
-      </c>
-      <c r="K44" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L44" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M44" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N44" s="8">
-        <v>0</v>
-      </c>
-      <c r="O44" s="8">
-        <v>0</v>
-      </c>
-      <c r="P44" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="8">
-        <v>117982.06368</v>
-      </c>
-      <c r="R44" s="8">
-        <v>6.5</v>
-      </c>
-      <c r="S44" s="8">
-        <v>0</v>
-      </c>
-      <c r="T44" s="8">
-        <v>0</v>
-      </c>
-      <c r="U44" s="8">
-        <v>0</v>
-      </c>
-      <c r="V44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="W44" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X44" s="1">
-        <v>14291</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24">
-      <c r="A45" s="7">
-        <v>43344</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J45" s="8">
-        <v>2555673.010176</v>
-      </c>
-      <c r="K45" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L45" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M45" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N45" s="8">
-        <v>-929335.640064</v>
-      </c>
-      <c r="O45" s="8">
-        <v>64</v>
-      </c>
-      <c r="P45" s="8">
-        <v>8</v>
-      </c>
-      <c r="Q45" s="8">
-        <v>0</v>
-      </c>
-      <c r="R45" s="8">
-        <v>0</v>
-      </c>
-      <c r="S45" s="8">
-        <v>0</v>
-      </c>
-      <c r="T45" s="8">
-        <v>0</v>
-      </c>
-      <c r="U45" s="8">
-        <v>0</v>
-      </c>
-      <c r="V45" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="W45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X45" s="1">
-        <v>14290</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24">
-      <c r="A46" s="7">
-        <v>43313</v>
-      </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J46" s="8">
-        <v>3639292.88736</v>
-      </c>
-      <c r="K46" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L46" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M46" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N46" s="8">
-        <v>0</v>
-      </c>
-      <c r="O46" s="8">
-        <v>0</v>
-      </c>
-      <c r="P46" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="8">
-        <v>154284.23712</v>
-      </c>
-      <c r="R46" s="8">
-        <v>8.5</v>
-      </c>
-      <c r="S46" s="8">
-        <v>0</v>
-      </c>
-      <c r="T46" s="8">
-        <v>0</v>
-      </c>
-      <c r="U46" s="8">
-        <v>0</v>
-      </c>
-      <c r="V46" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="W46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X46" s="1">
-        <v>14291</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24">
-      <c r="A47" s="7">
-        <v>43344</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J47" s="8">
-        <v>3584839.6272</v>
-      </c>
-      <c r="K47" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L47" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M47" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N47" s="8">
-        <v>0</v>
-      </c>
-      <c r="O47" s="8">
-        <v>0</v>
-      </c>
-      <c r="P47" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="8">
-        <v>99830.97696</v>
-      </c>
-      <c r="R47" s="8">
-        <v>5.5</v>
-      </c>
-      <c r="S47" s="8">
-        <v>0</v>
-      </c>
-      <c r="T47" s="8">
-        <v>0</v>
-      </c>
-      <c r="U47" s="8">
-        <v>0</v>
-      </c>
-      <c r="V47" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="W47" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X47" s="1">
-        <v>14290</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24">
-      <c r="A48" s="7">
-        <v>43374</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J48" s="8">
-        <v>3593915.17056</v>
-      </c>
-      <c r="K48" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L48" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M48" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N48" s="8">
-        <v>0</v>
-      </c>
-      <c r="O48" s="8">
-        <v>0</v>
-      </c>
-      <c r="P48" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="8">
-        <v>108906.52032</v>
-      </c>
-      <c r="R48" s="8">
-        <v>6</v>
-      </c>
-      <c r="S48" s="8">
-        <v>0</v>
-      </c>
-      <c r="T48" s="8">
-        <v>0</v>
-      </c>
-      <c r="U48" s="8">
-        <v>0</v>
-      </c>
-      <c r="V48" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="W48" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X48" s="1">
-        <v>14236</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24">
-      <c r="A49" s="7">
-        <v>43313</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="I49" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J49" s="8">
-        <v>3759090.059712</v>
-      </c>
-      <c r="K49" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L49" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M49" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N49" s="8">
-        <v>-116166.955008</v>
-      </c>
-      <c r="O49" s="8">
-        <v>8</v>
-      </c>
-      <c r="P49" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q49" s="8">
-        <v>390248.36448</v>
-      </c>
-      <c r="R49" s="8">
-        <v>21.5</v>
-      </c>
-      <c r="S49" s="8">
-        <v>0</v>
-      </c>
-      <c r="T49" s="8">
-        <v>0</v>
-      </c>
-      <c r="U49" s="8">
-        <v>0</v>
-      </c>
-      <c r="V49" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="W49" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X49" s="1">
-        <v>14291</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24">
-      <c r="A50" s="7">
-        <v>43344</v>
-      </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="I50" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J50" s="8">
-        <v>3877072.123392</v>
-      </c>
-      <c r="K50" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L50" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M50" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N50" s="8">
-        <v>-116166.955008</v>
-      </c>
-      <c r="O50" s="8">
-        <v>8</v>
-      </c>
-      <c r="P50" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q50" s="8">
-        <v>508230.42816</v>
-      </c>
-      <c r="R50" s="8">
-        <v>28</v>
-      </c>
-      <c r="S50" s="8">
-        <v>0</v>
-      </c>
-      <c r="T50" s="8">
-        <v>0</v>
-      </c>
-      <c r="U50" s="8">
-        <v>0</v>
-      </c>
-      <c r="V50" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="W50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X50" s="1">
-        <v>14290</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24">
-      <c r="A51" s="7">
-        <v>43374</v>
-      </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J51" s="8">
-        <v>3966012.44832</v>
-      </c>
-      <c r="K51" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L51" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M51" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N51" s="8">
-        <v>0</v>
-      </c>
-      <c r="O51" s="8">
-        <v>0</v>
-      </c>
-      <c r="P51" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="8">
-        <v>481003.79808</v>
-      </c>
-      <c r="R51" s="8">
-        <v>26.5</v>
-      </c>
-      <c r="S51" s="8">
-        <v>0</v>
-      </c>
-      <c r="T51" s="8">
-        <v>0</v>
-      </c>
-      <c r="U51" s="8">
-        <v>0</v>
-      </c>
-      <c r="V51" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="W51" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X51" s="1">
-        <v>14236</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24">
-      <c r="A52" s="7">
-        <v>43313</v>
-      </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I52" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J52" s="8">
-        <v>3252674.740224</v>
-      </c>
-      <c r="K52" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L52" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M52" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N52" s="8">
-        <v>-232333.910016</v>
-      </c>
-      <c r="O52" s="8">
-        <v>16</v>
-      </c>
-      <c r="P52" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q52" s="8">
-        <v>0</v>
-      </c>
-      <c r="R52" s="8">
-        <v>0</v>
-      </c>
-      <c r="S52" s="8">
-        <v>0</v>
-      </c>
-      <c r="T52" s="8">
-        <v>0</v>
-      </c>
-      <c r="U52" s="8">
-        <v>0</v>
-      </c>
-      <c r="V52" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="W52" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X52" s="1">
-        <v>14291</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24">
-      <c r="A53" s="7">
-        <v>43344</v>
-      </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I53" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J53" s="8">
-        <v>3368841.695232</v>
-      </c>
-      <c r="K53" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L53" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M53" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N53" s="8">
-        <v>-116166.955008</v>
-      </c>
-      <c r="O53" s="8">
-        <v>8</v>
-      </c>
-      <c r="P53" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q53" s="8">
-        <v>0</v>
-      </c>
-      <c r="R53" s="8">
-        <v>0</v>
-      </c>
-      <c r="S53" s="8">
-        <v>0</v>
-      </c>
-      <c r="T53" s="8">
-        <v>0</v>
-      </c>
-      <c r="U53" s="8">
-        <v>0</v>
-      </c>
-      <c r="V53" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="W53" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X53" s="1">
-        <v>14290</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24">
-      <c r="A54" s="7">
-        <v>43374</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I54" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J54" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="K54" s="8">
-        <v>2065440</v>
-      </c>
-      <c r="L54" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M54" s="8">
-        <v>3485008.65024</v>
-      </c>
-      <c r="N54" s="8">
-        <v>0</v>
-      </c>
-      <c r="O54" s="8">
-        <v>0</v>
-      </c>
-      <c r="P54" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="8">
-        <v>0</v>
-      </c>
-      <c r="R54" s="8">
-        <v>0</v>
-      </c>
-      <c r="S54" s="8">
-        <v>0</v>
-      </c>
-      <c r="T54" s="8">
-        <v>0</v>
-      </c>
-      <c r="U54" s="8">
-        <v>0</v>
-      </c>
-      <c r="V54" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W54" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X54" s="1">
-        <v>14236</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24">
-      <c r="A55" s="7">
-        <v>43374</v>
-      </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="I55" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J55" s="8">
-        <v>6967209.09829149</v>
-      </c>
-      <c r="K55" s="8">
-        <v>4424159.6152</v>
-      </c>
-      <c r="L55" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M55" s="8">
-        <v>7464866.88643072</v>
-      </c>
-      <c r="N55" s="8">
-        <v>-497657.788139233</v>
-      </c>
-      <c r="O55" s="8">
-        <v>16</v>
-      </c>
-      <c r="P55" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q55" s="8">
-        <v>0</v>
-      </c>
-      <c r="R55" s="8">
-        <v>0</v>
-      </c>
-      <c r="S55" s="8">
-        <v>0</v>
-      </c>
-      <c r="T55" s="8">
-        <v>0</v>
-      </c>
-      <c r="U55" s="8">
-        <v>0</v>
-      </c>
-      <c r="V55" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="W55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X55" s="1">
-        <v>14236</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24">
-      <c r="A56" s="7">
-        <v>43313</v>
-      </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8">
-        <v>1577</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="I56" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="J56" s="8">
-        <v>7464867.47136</v>
-      </c>
-      <c r="K56" s="8">
-        <v>4424160</v>
-      </c>
-      <c r="L56" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M56" s="8">
-        <v>7464867.47136</v>
-      </c>
-      <c r="N56" s="8">
-        <v>0</v>
-      </c>
-      <c r="O56" s="8">
-        <v>0</v>
-      </c>
-      <c r="P56" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="8">
-        <v>0</v>
-      </c>
-      <c r="R56" s="8">
-        <v>0</v>
-      </c>
-      <c r="S56" s="8">
-        <v>0</v>
-      </c>
-      <c r="T56" s="8">
-        <v>0</v>
-      </c>
-      <c r="U56" s="8">
-        <v>0</v>
-      </c>
-      <c r="V56" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X56" s="1">
-        <v>14291</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57"/>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
-      <c r="J57"/>
-      <c r="K57"/>
-      <c r="L57"/>
-      <c r="M57"/>
-      <c r="N57"/>
-      <c r="O57"/>
-      <c r="P57"/>
-      <c r="Q57"/>
-      <c r="R57"/>
-      <c r="S57"/>
-      <c r="T57"/>
-      <c r="U57"/>
-      <c r="V57"/>
-      <c r="W57"/>
-      <c r="X57"/>
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Revert "28-11-2018: Commit con programa de secop y comentarios sobre r para corregir"
This reverts commit 052ba9a4d753956103fa2b6ed0061dca21d49d1e.
</commit_message>
<xml_diff>
--- a/syncfusion_payc/syncfusion_payc/VISTA_DETALLE_ADJUNTOS_PERS/adjuntosfactura/Adjunto_11899.xlsx
+++ b/syncfusion_payc/syncfusion_payc/VISTA_DETALLE_ADJUNTOS_PERS/adjuntosfactura/Adjunto_11899.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94" count="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117" count="448">
   <si>
     <t>Periodo Facturación</t>
   </si>
@@ -140,6 +140,15 @@
     <t>TIPO NOVEDAD:INCAPACIDAD - FECHA INICIO:Oct  5 2018 12:00AM - FECHA FIN:Oct  6 2018 12:00AM</t>
   </si>
   <si>
+    <t>RESIDENTE DE INSTALACIONES</t>
+  </si>
+  <si>
+    <t>JAIRO HERNAN WILLS RIANO</t>
+  </si>
+  <si>
+    <t>nov. 01 2017</t>
+  </si>
+  <si>
     <t>RESIDENTE ADMINISTRATIVO</t>
   </si>
   <si>
@@ -206,6 +215,18 @@
     <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM</t>
   </si>
   <si>
+    <t>MAREYEY FIQUE MORENO</t>
+  </si>
+  <si>
+    <t>ene. 02 2018</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM</t>
+  </si>
+  <si>
     <t>RESIDENTE SOTANOS</t>
   </si>
   <si>
@@ -230,6 +251,15 @@
     <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  5 2018 12:00AM</t>
   </si>
   <si>
+    <t>RESIDENTE URBANISMO</t>
+  </si>
+  <si>
+    <t>LEONARDO ALBERTO DUSSAN GARCIA</t>
+  </si>
+  <si>
+    <t>ene. 24 2017</t>
+  </si>
+  <si>
     <t>RESIDENTE TORRE 1</t>
   </si>
   <si>
@@ -239,12 +269,27 @@
     <t>ago. 09 2016</t>
   </si>
   <si>
-    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM</t>
-  </si>
-  <si>
     <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  8 2018 12:00AM</t>
   </si>
   <si>
+    <t>INSPECTOR SOTANOS</t>
+  </si>
+  <si>
+    <t>LUIS ORLANDO CARDOZO ZORRO</t>
+  </si>
+  <si>
+    <t>jun. 11 2017</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  2 2018  2:30AM, TIPO NOVEDAD:HORAS_EXTRAS_NOCTURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  2:30AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  2 2018 12:00AM</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep 10 2018 12:00AM</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  1 2018  2:30PM</t>
+  </si>
+  <si>
     <t>INSPECTOR COMERCIO</t>
   </si>
   <si>
@@ -291,6 +336,30 @@
   </si>
   <si>
     <t>TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  2 2018  2:30AM</t>
+  </si>
+  <si>
+    <t>INSPECTOR TORRE 2</t>
+  </si>
+  <si>
+    <t>JORGE EDUARDO YAZO PATARROYO</t>
+  </si>
+  <si>
+    <t>oct. 12 2016</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM</t>
+  </si>
+  <si>
+    <t>RESIDENTE AMBIENTAL</t>
+  </si>
+  <si>
+    <t>CLAUDIA MARCELA DIAZ BARBOSA</t>
+  </si>
+  <si>
+    <t>oct. 01 2018</t>
+  </si>
+  <si>
+    <t>TIPO NOVEDAD:INCAPACIDAD - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  2 2018 12:00AM</t>
   </si>
   <si>
     <t>PAMELA OCAMPO GRISALES</t>
@@ -606,9 +675,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:d1p1="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" d1p1:id="rId1" refreshedBy="DefaultAppPool" refreshedDate="43430.674432002314" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" refreshOnLoad="1" recordCount="0">
+<pivotCacheDefinition xmlns:d1p1="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" d1p1:id="rId1" refreshedBy="DefaultAppPool" refreshedDate="43427.384906631945" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" refreshOnLoad="1" recordCount="0">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A3:X40" sheet="BASE DE DATOS"/>
+    <worksheetSource ref="A3:X56" sheet="BASE DE DATOS"/>
   </cacheSource>
   <cacheFields count="24">
     <cacheField name="Periodo Facturación" numFmtId="0">
@@ -642,31 +711,42 @@
       <sharedItems>
         <s v="COORDINADOR"/>
         <s v="DIRECTOR"/>
+        <s v="RESIDENTE DE INSTALACIONES"/>
         <s v="RESIDENTE ADMINISTRATIVO"/>
         <s v="AUXILIAR ADMINISTRATIVO"/>
         <s v="RESIDENTE SOTANOS"/>
         <s v="RESIDENTE DE COMERCIO "/>
+        <s v="RESIDENTE URBANISMO"/>
         <s v="RESIDENTE TORRE 1"/>
+        <s v="INSPECTOR SOTANOS"/>
         <s v="INSPECTOR COMERCIO"/>
         <s v="INSPECTOR TORRE 1"/>
         <s v="INSPECTOR TORRE 1 ESTRUCTURA"/>
+        <s v="INSPECTOR TORRE 2"/>
+        <s v="RESIDENTE AMBIENTAL"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Nombre colaborador / Item" numFmtId="0">
       <sharedItems>
         <s v="CARLOS ALFREDO NEIRA GRAJALES"/>
         <s v="JORGE ENRIQUE CASSALETT BUSTILLO"/>
+        <s v="JAIRO HERNAN WILLS RIANO"/>
         <s v="MARIA PIEDAD ESPINOSA VIRGUEZ"/>
         <s v="LORNA ROCIO SANCHEZ ROLDAN"/>
         <s v="YEIMY KATERINE PIRAJAN APARICIO"/>
         <s v="RUBY TATIANA PERDIGON DE LOS RIOS"/>
         <s v="SEBASTIAN FELIPE DIAZ RIVEROS"/>
+        <s v="MAREYEY FIQUE MORENO"/>
         <s v="DIEGO ANDRES CERINZA HUERTAS"/>
         <s v="JENNY CONSTANZA CONTENTO FUENTES"/>
+        <s v="LEONARDO ALBERTO DUSSAN GARCIA"/>
         <s v="JOHAN GABRIEL QUIROGA RODRIGUEZ"/>
+        <s v="LUIS ORLANDO CARDOZO ZORRO"/>
         <s v="VICTOR MANUEL AVENDANO LEON"/>
         <s v="EBERTO LIBARDO BRAVO MENESES"/>
         <s v="PEDRO PABLO HERRERA SALDARRIAGA"/>
+        <s v="JORGE EDUARDO YAZO PATARROYO"/>
+        <s v="CLAUDIA MARCELA DIAZ BARBOSA"/>
         <s v="PAMELA OCAMPO GRISALES"/>
       </sharedItems>
     </cacheField>
@@ -674,17 +754,23 @@
       <sharedItems>
         <s v="may. 01 2018"/>
         <s v="sep. 01 2016"/>
+        <s v="nov. 01 2017"/>
         <s v="ago. 15 2016"/>
         <s v="sep. 26 2017"/>
         <s v="feb. 13 2017"/>
         <s v="oct. 25 2016"/>
         <s v="dic. 11 2016"/>
+        <s v="ene. 02 2018"/>
         <s v="ene. 08 2016"/>
         <s v="ago. 24 2017"/>
+        <s v="ene. 24 2017"/>
         <s v="ago. 09 2016"/>
+        <s v="jun. 11 2017"/>
         <s v="oct. 10 2017"/>
         <s v="ene. 14 2015"/>
         <s v="sep. 16 2015"/>
+        <s v="oct. 12 2016"/>
+        <s v="oct. 01 2018"/>
         <s v="oct. 20 2016"/>
       </sharedItems>
     </cacheField>
@@ -702,6 +788,7 @@
         <n v="9003523.9424"/>
         <n v="8643382.984704"/>
         <n v="10083946.815488"/>
+        <n v="9084536.64768"/>
         <n v="4820051.238912"/>
         <n v="4303617.1776"/>
         <n v="5164340.61312"/>
@@ -714,12 +801,20 @@
         <n v="2016602.185728"/>
         <n v="3558709.73952"/>
         <n v="3202838.765568"/>
+        <n v="3440086.081536"/>
+        <n v="3321462.423552"/>
         <n v="5971893.4576708"/>
         <n v="7464866.8220885"/>
         <n v="6220722.35174042"/>
+        <n v="6106661.6832"/>
+        <n v="5896087.1424"/>
+        <n v="6317236.224"/>
         <n v="7216038.555648"/>
         <n v="5474236.145664"/>
         <n v="7464867.47136"/>
+        <n v="3797207.341824"/>
+        <n v="2758965.18144"/>
+        <n v="3748199.40768"/>
         <n v="3602990.71392"/>
         <n v="2555673.010176"/>
         <n v="3639292.88736"/>
@@ -728,15 +823,21 @@
         <n v="3759090.059712"/>
         <n v="3877072.123392"/>
         <n v="3966012.44832"/>
+        <n v="3252674.740224"/>
+        <n v="3368841.695232"/>
+        <n v="3485008.65024"/>
+        <n v="6967209.09829149"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Salario básico" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="1853904"/>
         <n v="6403280"/>
+        <n v="5384080"/>
         <n v="3060720"/>
         <n v="2109120"/>
         <n v="4424159.6152"/>
+        <n v="3744000"/>
         <n v="4424160"/>
         <n v="2065440"/>
       </sharedItems>
@@ -751,12 +852,15 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="3378331.58787072"/>
         <n v="10804228.73088"/>
+        <n v="9084536.64768"/>
         <n v="5164340.61312"/>
         <n v="1205012.809728"/>
         <n v="3558709.73952"/>
         <n v="7464866.8220885"/>
+        <n v="6317236.224"/>
         <n v="7464867.47136"/>
         <n v="3485008.65024"/>
+        <n v="7464866.88643072"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Descuentos (Novedades)" numFmtId="0">
@@ -774,12 +878,19 @@
         <n v="-1067612.921856"/>
         <n v="-1542107.553792"/>
         <n v="-355870.973952"/>
+        <n v="-118623.657984"/>
+        <n v="-237247.315968"/>
         <n v="-1492973.3644177"/>
         <n v="-1244144.47034808"/>
+        <n v="-210574.5408"/>
+        <n v="-421149.0816"/>
         <n v="-248828.915712"/>
         <n v="-1990631.325696"/>
+        <n v="-232333.910016"/>
+        <n v="-1161669.55008"/>
         <n v="-929335.640064"/>
         <n v="-116166.955008"/>
+        <n v="-497657.788139233"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Total horas novedades" numFmtId="0">
@@ -794,6 +905,7 @@
         <n v="72"/>
         <n v="104"/>
         <n v="8"/>
+        <n v="80"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Total días novedades" numFmtId="0">
@@ -808,11 +920,15 @@
         <n v="9"/>
         <n v="13"/>
         <n v="1"/>
+        <n v="10"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Horas Extra" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="0"/>
+        <n v="544532.6016"/>
+        <n v="435626.08128"/>
+        <n v="263190.75744"/>
         <n v="117982.06368"/>
         <n v="154284.23712"/>
         <n v="99830.97696"/>
@@ -825,18 +941,21 @@
     <cacheField name="HE Diurnas" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="0"/>
+        <n v="26.5"/>
+        <n v="24"/>
+        <n v="14.5"/>
         <n v="6.5"/>
         <n v="8.5"/>
         <n v="5.5"/>
         <n v="6"/>
         <n v="21.5"/>
         <n v="28"/>
-        <n v="26.5"/>
       </sharedItems>
     </cacheField>
     <cacheField name="HE Nocturnas" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="0">
         <n v="0"/>
+        <n v="2.5"/>
       </sharedItems>
     </cacheField>
     <cacheField name="HE Festivas Diurnas" numFmtId="0">
@@ -850,7 +969,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Detalle Novedades" numFmtId="0">
-      <sharedItems>
+      <sharedItems longText="1">
         <s v="SIN NOVEDADES ago. 2018"/>
         <s v="SIN NOVEDADES sep. 2018"/>
         <s v="SIN NOVEDADES oct. 2018"/>
@@ -865,10 +984,14 @@
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  9 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep 12 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM"/>
+        <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM"/>
+        <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  6 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  5 2018 12:00AM"/>
-        <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  8 2018 12:00AM"/>
+        <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  2 2018  2:30AM, TIPO NOVEDAD:HORAS_EXTRAS_NOCTURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  2:30AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  2 2018 12:00AM"/>
+        <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018 12:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep 10 2018 12:00AM"/>
+        <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  1 2018  2:30PM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  6:30AM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  8:30AM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018  5:30AM"/>
@@ -876,6 +999,8 @@
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018  9:30PM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Aug  1 2018 12:00AM - FECHA FIN:Aug  1 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  2 2018  4:00AM, TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM"/>
         <s v="TIPO NOVEDAD:HORAS_EXTRAS_DIURNAS - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  2 2018  2:30AM"/>
+        <s v="TIPO NOVEDAD:AUSENCIA INJUSTIFICADA - FECHA INICIO:Sep  1 2018 12:00AM - FECHA FIN:Sep  1 2018 12:00AM"/>
+        <s v="TIPO NOVEDAD:INCAPACIDAD - FECHA INICIO:Oct  1 2018 12:00AM - FECHA FIN:Oct  2 2018 12:00AM"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Dedicación" numFmtId="0">
@@ -919,52 +1044,69 @@
     </pivotField>
     <pivotField axis="axisRow" outline="0" compact="0" showAll="0" defaultSubtotal="0">
       <items>
-        <item x="3"/>
+        <item x="4"/>
         <item x="0"/>
         <item x="1"/>
-        <item x="7"/>
-        <item x="8"/>
+        <item x="10"/>
         <item x="9"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item x="14"/>
+        <item x="6"/>
         <item x="2"/>
         <item x="5"/>
-        <item x="4"/>
-        <item x="6"/>
+        <item x="8"/>
+        <item x="7"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" outline="0" compact="0" showAll="0" defaultSubtotal="0">
       <items>
         <item x="0"/>
+        <item x="18"/>
+        <item x="9"/>
+        <item x="15"/>
+        <item x="2"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="17"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="19"/>
+        <item x="16"/>
+        <item x="6"/>
         <item x="7"/>
-        <item x="11"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="13"/>
-        <item x="12"/>
+        <item x="14"/>
         <item x="5"/>
-        <item x="6"/>
-        <item x="10"/>
-        <item x="4"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" outline="0" compact="0" showAll="0" defaultSubtotal="0">
       <items>
-        <item x="9"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="11"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="10"/>
-        <item x="13"/>
-        <item x="5"/>
-        <item x="1"/>
         <item x="12"/>
         <item x="3"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="15"/>
+        <item x="11"/>
+        <item x="5"/>
+        <item x="13"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="18"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="16"/>
+        <item x="4"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" outline="0" compact="0" showAll="0" defaultSubtotal="0">
@@ -1163,7 +1305,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:X57"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -1758,25 +1900,25 @@
         <v>29</v>
       </c>
       <c r="J10" s="8">
-        <v>4820051.238912</v>
+        <v>9084536.64768</v>
       </c>
       <c r="K10" s="8">
-        <v>3060720</v>
+        <v>5384080</v>
       </c>
       <c r="L10" s="8">
         <v>0.5</v>
       </c>
       <c r="M10" s="8">
-        <v>5164340.61312</v>
+        <v>9084536.64768</v>
       </c>
       <c r="N10" s="8">
-        <v>-344289.374208</v>
+        <v>0</v>
       </c>
       <c r="O10" s="8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="P10" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="8">
         <v>0</v>
@@ -1794,7 +1936,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>31</v>
@@ -1830,25 +1972,25 @@
         <v>29</v>
       </c>
       <c r="J11" s="8">
-        <v>4303617.1776</v>
+        <v>9084536.64768</v>
       </c>
       <c r="K11" s="8">
-        <v>3060720</v>
+        <v>5384080</v>
       </c>
       <c r="L11" s="8">
         <v>0.5</v>
       </c>
       <c r="M11" s="8">
-        <v>5164340.61312</v>
+        <v>9084536.64768</v>
       </c>
       <c r="N11" s="8">
-        <v>-860723.43552</v>
+        <v>0</v>
       </c>
       <c r="O11" s="8">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="P11" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="8">
         <v>0</v>
@@ -1866,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>31</v>
@@ -1902,16 +2044,16 @@
         <v>29</v>
       </c>
       <c r="J12" s="8">
-        <v>5164340.61312</v>
+        <v>9084536.64768</v>
       </c>
       <c r="K12" s="8">
-        <v>3060720</v>
+        <v>5384080</v>
       </c>
       <c r="L12" s="8">
         <v>0.5</v>
       </c>
       <c r="M12" s="8">
-        <v>5164340.61312</v>
+        <v>9084536.64768</v>
       </c>
       <c r="N12" s="8">
         <v>0</v>
@@ -1962,19 +2104,19 @@
         <v>25</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="I13" s="8" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="J13" s="8">
-        <v>4647906.551808</v>
+        <v>4820051.238912</v>
       </c>
       <c r="K13" s="8">
         <v>3060720</v>
@@ -1986,13 +2128,13 @@
         <v>5164340.61312</v>
       </c>
       <c r="N13" s="8">
-        <v>-516434.061312</v>
+        <v>-344289.374208</v>
       </c>
       <c r="O13" s="8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="P13" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="8">
         <v>0</v>
@@ -2010,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>31</v>
@@ -2034,19 +2176,19 @@
         <v>25</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="I14" s="8" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="J14" s="8">
-        <v>4131472.490496</v>
+        <v>4303617.1776</v>
       </c>
       <c r="K14" s="8">
         <v>3060720</v>
@@ -2058,13 +2200,13 @@
         <v>5164340.61312</v>
       </c>
       <c r="N14" s="8">
-        <v>-1032868.122624</v>
+        <v>-860723.43552</v>
       </c>
       <c r="O14" s="8">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="P14" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="8">
         <v>0</v>
@@ -2082,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>31</v>
@@ -2106,19 +2248,19 @@
         <v>25</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="I15" s="8" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="J15" s="8">
-        <v>1205012.809728</v>
+        <v>5164340.61312</v>
       </c>
       <c r="K15" s="8">
         <v>3060720</v>
@@ -2127,7 +2269,7 @@
         <v>0.5</v>
       </c>
       <c r="M15" s="8">
-        <v>1205012.809728</v>
+        <v>5164340.61312</v>
       </c>
       <c r="N15" s="8">
         <v>0</v>
@@ -2178,19 +2320,19 @@
         <v>25</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="J16" s="8">
-        <v>3787183.116288</v>
+        <v>4647906.551808</v>
       </c>
       <c r="K16" s="8">
         <v>3060720</v>
@@ -2202,13 +2344,13 @@
         <v>5164340.61312</v>
       </c>
       <c r="N16" s="8">
-        <v>-1377157.496832</v>
+        <v>-516434.061312</v>
       </c>
       <c r="O16" s="8">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="P16" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q16" s="8">
         <v>0</v>
@@ -2226,7 +2368,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W16" s="1" t="s">
         <v>31</v>
@@ -2250,19 +2392,19 @@
         <v>25</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="I17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="J17" s="8">
-        <v>3270749.054976</v>
+        <v>4131472.490496</v>
       </c>
       <c r="K17" s="8">
         <v>3060720</v>
@@ -2274,13 +2416,13 @@
         <v>5164340.61312</v>
       </c>
       <c r="N17" s="8">
-        <v>-1893591.558144</v>
+        <v>-1032868.122624</v>
       </c>
       <c r="O17" s="8">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="P17" s="8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="Q17" s="8">
         <v>0</v>
@@ -2298,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>31</v>
@@ -2309,7 +2451,7 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" s="7">
-        <v>43313</v>
+        <v>43374</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8">
@@ -2322,37 +2464,37 @@
         <v>25</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J18" s="8">
-        <v>2491096.817664</v>
+        <v>1205012.809728</v>
       </c>
       <c r="K18" s="8">
-        <v>2109120</v>
+        <v>3060720</v>
       </c>
       <c r="L18" s="8">
         <v>0.5</v>
       </c>
       <c r="M18" s="8">
-        <v>3558709.73952</v>
+        <v>1205012.809728</v>
       </c>
       <c r="N18" s="8">
-        <v>-1067612.921856</v>
+        <v>0</v>
       </c>
       <c r="O18" s="8">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="P18" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="8">
         <v>0</v>
@@ -2370,18 +2512,18 @@
         <v>0</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X18" s="1">
-        <v>14291</v>
+        <v>14236</v>
       </c>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="7">
-        <v>43344</v>
+        <v>43313</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8">
@@ -2394,37 +2536,37 @@
         <v>25</v>
       </c>
       <c r="F19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="J19" s="8">
-        <v>2016602.185728</v>
+        <v>3787183.116288</v>
       </c>
       <c r="K19" s="8">
-        <v>2109120</v>
+        <v>3060720</v>
       </c>
       <c r="L19" s="8">
         <v>0.5</v>
       </c>
       <c r="M19" s="8">
-        <v>3558709.73952</v>
+        <v>5164340.61312</v>
       </c>
       <c r="N19" s="8">
-        <v>-1542107.553792</v>
+        <v>-1377157.496832</v>
       </c>
       <c r="O19" s="8">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="P19" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="8">
         <v>0</v>
@@ -2442,18 +2584,18 @@
         <v>0</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="W19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X19" s="1">
-        <v>14290</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="7">
-        <v>43313</v>
+        <v>43344</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8">
@@ -2466,37 +2608,37 @@
         <v>25</v>
       </c>
       <c r="F20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="J20" s="8">
-        <v>3558709.73952</v>
+        <v>3270749.054976</v>
       </c>
       <c r="K20" s="8">
-        <v>2109120</v>
+        <v>3060720</v>
       </c>
       <c r="L20" s="8">
         <v>0.5</v>
       </c>
       <c r="M20" s="8">
-        <v>3558709.73952</v>
+        <v>5164340.61312</v>
       </c>
       <c r="N20" s="8">
-        <v>0</v>
+        <v>-1893591.558144</v>
       </c>
       <c r="O20" s="8">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="P20" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Q20" s="8">
         <v>0</v>
@@ -2514,18 +2656,18 @@
         <v>0</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X20" s="1">
-        <v>14291</v>
+        <v>14290</v>
       </c>
     </row>
     <row r="21" spans="1:24">
       <c r="A21" s="7">
-        <v>43344</v>
+        <v>43313</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8">
@@ -2538,19 +2680,19 @@
         <v>25</v>
       </c>
       <c r="F21" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="J21" s="8">
-        <v>3202838.765568</v>
+        <v>2491096.817664</v>
       </c>
       <c r="K21" s="8">
         <v>2109120</v>
@@ -2562,13 +2704,13 @@
         <v>3558709.73952</v>
       </c>
       <c r="N21" s="8">
-        <v>-355870.973952</v>
+        <v>-1067612.921856</v>
       </c>
       <c r="O21" s="8">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="P21" s="8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="Q21" s="8">
         <v>0</v>
@@ -2586,18 +2728,18 @@
         <v>0</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X21" s="1">
-        <v>14290</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="22" spans="1:24">
       <c r="A22" s="7">
-        <v>43374</v>
+        <v>43344</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8">
@@ -2610,19 +2752,19 @@
         <v>25</v>
       </c>
       <c r="F22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="J22" s="8">
-        <v>3558709.73952</v>
+        <v>2016602.185728</v>
       </c>
       <c r="K22" s="8">
         <v>2109120</v>
@@ -2634,13 +2776,13 @@
         <v>3558709.73952</v>
       </c>
       <c r="N22" s="8">
-        <v>0</v>
+        <v>-1542107.553792</v>
       </c>
       <c r="O22" s="8">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="P22" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="Q22" s="8">
         <v>0</v>
@@ -2658,13 +2800,13 @@
         <v>0</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="W22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X22" s="1">
-        <v>14236</v>
+        <v>14290</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -2682,37 +2824,37 @@
         <v>25</v>
       </c>
       <c r="F23" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="H23" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J23" s="8">
-        <v>5971893.4576708</v>
+        <v>3558709.73952</v>
       </c>
       <c r="K23" s="8">
-        <v>4424159.6152</v>
+        <v>2109120</v>
       </c>
       <c r="L23" s="8">
         <v>0.5</v>
       </c>
       <c r="M23" s="8">
-        <v>7464866.8220885</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N23" s="8">
-        <v>-1492973.3644177</v>
+        <v>0</v>
       </c>
       <c r="O23" s="8">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="P23" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="8">
         <v>0</v>
@@ -2730,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="W23" s="1" t="s">
         <v>31</v>
@@ -2754,37 +2896,37 @@
         <v>25</v>
       </c>
       <c r="F24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="H24" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J24" s="8">
-        <v>7464866.8220885</v>
+        <v>3202838.765568</v>
       </c>
       <c r="K24" s="8">
-        <v>4424159.6152</v>
+        <v>2109120</v>
       </c>
       <c r="L24" s="8">
         <v>0.5</v>
       </c>
       <c r="M24" s="8">
-        <v>7464866.8220885</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N24" s="8">
-        <v>0</v>
+        <v>-355870.973952</v>
       </c>
       <c r="O24" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="P24" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q24" s="8">
         <v>0</v>
@@ -2802,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="W24" s="1" t="s">
         <v>31</v>
@@ -2826,28 +2968,28 @@
         <v>25</v>
       </c>
       <c r="F25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="H25" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J25" s="8">
-        <v>7464866.8220885</v>
+        <v>3558709.73952</v>
       </c>
       <c r="K25" s="8">
-        <v>4424159.6152</v>
+        <v>2109120</v>
       </c>
       <c r="L25" s="8">
         <v>0.5</v>
       </c>
       <c r="M25" s="8">
-        <v>7464866.8220885</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N25" s="8">
         <v>0</v>
@@ -2898,37 +3040,37 @@
         <v>25</v>
       </c>
       <c r="F26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J26" s="8">
-        <v>6220722.35174042</v>
+        <v>3440086.081536</v>
       </c>
       <c r="K26" s="8">
-        <v>4424159.6152</v>
+        <v>2109120</v>
       </c>
       <c r="L26" s="8">
         <v>0.5</v>
       </c>
       <c r="M26" s="8">
-        <v>7464866.8220885</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N26" s="8">
-        <v>-1244144.47034808</v>
+        <v>-118623.657984</v>
       </c>
       <c r="O26" s="8">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="P26" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="8">
         <v>0</v>
@@ -2946,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W26" s="1" t="s">
         <v>31</v>
@@ -2970,37 +3112,37 @@
         <v>25</v>
       </c>
       <c r="F27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J27" s="8">
-        <v>7464866.8220885</v>
+        <v>3321462.423552</v>
       </c>
       <c r="K27" s="8">
-        <v>4424159.6152</v>
+        <v>2109120</v>
       </c>
       <c r="L27" s="8">
         <v>0.5</v>
       </c>
       <c r="M27" s="8">
-        <v>7464866.8220885</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N27" s="8">
-        <v>0</v>
+        <v>-237247.315968</v>
       </c>
       <c r="O27" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P27" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q27" s="8">
         <v>0</v>
@@ -3018,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="W27" s="1" t="s">
         <v>31</v>
@@ -3042,28 +3184,28 @@
         <v>25</v>
       </c>
       <c r="F28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J28" s="8">
-        <v>7464866.8220885</v>
+        <v>3558709.73952</v>
       </c>
       <c r="K28" s="8">
-        <v>4424159.6152</v>
+        <v>2109120</v>
       </c>
       <c r="L28" s="8">
         <v>0.5</v>
       </c>
       <c r="M28" s="8">
-        <v>7464866.8220885</v>
+        <v>3558709.73952</v>
       </c>
       <c r="N28" s="8">
         <v>0</v>
@@ -3114,37 +3256,37 @@
         <v>25</v>
       </c>
       <c r="F29" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="H29" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J29" s="8">
-        <v>7216038.555648</v>
+        <v>5971893.4576708</v>
       </c>
       <c r="K29" s="8">
-        <v>4424160</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L29" s="8">
         <v>0.5</v>
       </c>
       <c r="M29" s="8">
-        <v>7464867.47136</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N29" s="8">
-        <v>-248828.915712</v>
+        <v>-1492973.3644177</v>
       </c>
       <c r="O29" s="8">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="P29" s="8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q29" s="8">
         <v>0</v>
@@ -3162,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W29" s="1" t="s">
         <v>31</v>
@@ -3186,37 +3328,37 @@
         <v>25</v>
       </c>
       <c r="F30" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="H30" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J30" s="8">
-        <v>5474236.145664</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="K30" s="8">
-        <v>4424160</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L30" s="8">
         <v>0.5</v>
       </c>
       <c r="M30" s="8">
-        <v>7464867.47136</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N30" s="8">
-        <v>-1990631.325696</v>
+        <v>0</v>
       </c>
       <c r="O30" s="8">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="P30" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="8">
         <v>0</v>
@@ -3234,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="W30" s="1" t="s">
         <v>31</v>
@@ -3258,28 +3400,28 @@
         <v>25</v>
       </c>
       <c r="F31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="H31" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J31" s="8">
-        <v>7464867.47136</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="K31" s="8">
-        <v>4424160</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L31" s="8">
         <v>0.5</v>
       </c>
       <c r="M31" s="8">
-        <v>7464867.47136</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N31" s="8">
         <v>0</v>
@@ -3330,43 +3472,43 @@
         <v>25</v>
       </c>
       <c r="F32" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="I32" s="8" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="J32" s="8">
-        <v>3602990.71392</v>
+        <v>6220722.35174042</v>
       </c>
       <c r="K32" s="8">
-        <v>2065440</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L32" s="8">
         <v>0.5</v>
       </c>
       <c r="M32" s="8">
-        <v>3485008.65024</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N32" s="8">
-        <v>0</v>
+        <v>-1244144.47034808</v>
       </c>
       <c r="O32" s="8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P32" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q32" s="8">
-        <v>117982.06368</v>
+        <v>0</v>
       </c>
       <c r="R32" s="8">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="S32" s="8">
         <v>0</v>
@@ -3378,7 +3520,7 @@
         <v>0</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="W32" s="1" t="s">
         <v>31</v>
@@ -3402,37 +3544,37 @@
         <v>25</v>
       </c>
       <c r="F33" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="I33" s="8" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="J33" s="8">
-        <v>2555673.010176</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="K33" s="8">
-        <v>2065440</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L33" s="8">
         <v>0.5</v>
       </c>
       <c r="M33" s="8">
-        <v>3485008.65024</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N33" s="8">
-        <v>-929335.640064</v>
+        <v>0</v>
       </c>
       <c r="O33" s="8">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="P33" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="8">
         <v>0</v>
@@ -3450,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>31</v>
@@ -3461,7 +3603,7 @@
     </row>
     <row r="34" spans="1:24">
       <c r="A34" s="7">
-        <v>43313</v>
+        <v>43374</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8">
@@ -3474,28 +3616,28 @@
         <v>25</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J34" s="8">
-        <v>3639292.88736</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="K34" s="8">
-        <v>2065440</v>
+        <v>4424159.6152</v>
       </c>
       <c r="L34" s="8">
         <v>0.5</v>
       </c>
       <c r="M34" s="8">
-        <v>3485008.65024</v>
+        <v>7464866.8220885</v>
       </c>
       <c r="N34" s="8">
         <v>0</v>
@@ -3507,10 +3649,10 @@
         <v>0</v>
       </c>
       <c r="Q34" s="8">
-        <v>154284.23712</v>
+        <v>0</v>
       </c>
       <c r="R34" s="8">
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="S34" s="8">
         <v>0</v>
@@ -3522,18 +3664,18 @@
         <v>0</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X34" s="1">
-        <v>14291</v>
+        <v>14236</v>
       </c>
     </row>
     <row r="35" spans="1:24">
       <c r="A35" s="7">
-        <v>43344</v>
+        <v>43313</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8">
@@ -3546,43 +3688,43 @@
         <v>25</v>
       </c>
       <c r="F35" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J35" s="8">
-        <v>3584839.6272</v>
+        <v>6106661.6832</v>
       </c>
       <c r="K35" s="8">
-        <v>2065440</v>
+        <v>3744000</v>
       </c>
       <c r="L35" s="8">
         <v>0.5</v>
       </c>
       <c r="M35" s="8">
-        <v>3485008.65024</v>
+        <v>6317236.224</v>
       </c>
       <c r="N35" s="8">
-        <v>0</v>
+        <v>-210574.5408</v>
       </c>
       <c r="O35" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P35" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q35" s="8">
-        <v>99830.97696</v>
+        <v>0</v>
       </c>
       <c r="R35" s="8">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="S35" s="8">
         <v>0</v>
@@ -3594,18 +3736,18 @@
         <v>0</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="W35" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X35" s="1">
-        <v>14290</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="36" spans="1:24">
       <c r="A36" s="7">
-        <v>43374</v>
+        <v>43344</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8">
@@ -3618,43 +3760,43 @@
         <v>25</v>
       </c>
       <c r="F36" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J36" s="8">
-        <v>3593915.17056</v>
+        <v>5896087.1424</v>
       </c>
       <c r="K36" s="8">
-        <v>2065440</v>
+        <v>3744000</v>
       </c>
       <c r="L36" s="8">
         <v>0.5</v>
       </c>
       <c r="M36" s="8">
-        <v>3485008.65024</v>
+        <v>6317236.224</v>
       </c>
       <c r="N36" s="8">
-        <v>0</v>
+        <v>-421149.0816</v>
       </c>
       <c r="O36" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P36" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q36" s="8">
-        <v>108906.52032</v>
+        <v>0</v>
       </c>
       <c r="R36" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S36" s="8">
         <v>0</v>
@@ -3666,18 +3808,18 @@
         <v>0</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="W36" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X36" s="1">
-        <v>14236</v>
+        <v>14290</v>
       </c>
     </row>
     <row r="37" spans="1:24">
       <c r="A37" s="7">
-        <v>43313</v>
+        <v>43374</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8">
@@ -3690,43 +3832,43 @@
         <v>25</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J37" s="8">
-        <v>3759090.059712</v>
+        <v>6317236.224</v>
       </c>
       <c r="K37" s="8">
-        <v>2065440</v>
+        <v>3744000</v>
       </c>
       <c r="L37" s="8">
         <v>0.5</v>
       </c>
       <c r="M37" s="8">
-        <v>3485008.65024</v>
+        <v>6317236.224</v>
       </c>
       <c r="N37" s="8">
-        <v>-116166.955008</v>
+        <v>0</v>
       </c>
       <c r="O37" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P37" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="8">
-        <v>390248.36448</v>
+        <v>0</v>
       </c>
       <c r="R37" s="8">
-        <v>21.5</v>
+        <v>0</v>
       </c>
       <c r="S37" s="8">
         <v>0</v>
@@ -3738,18 +3880,18 @@
         <v>0</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="W37" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X37" s="1">
-        <v>14291</v>
+        <v>14236</v>
       </c>
     </row>
     <row r="38" spans="1:24">
       <c r="A38" s="7">
-        <v>43344</v>
+        <v>43313</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8">
@@ -3762,31 +3904,31 @@
         <v>25</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J38" s="8">
-        <v>3877072.123392</v>
+        <v>7216038.555648</v>
       </c>
       <c r="K38" s="8">
-        <v>2065440</v>
+        <v>4424160</v>
       </c>
       <c r="L38" s="8">
         <v>0.5</v>
       </c>
       <c r="M38" s="8">
-        <v>3485008.65024</v>
+        <v>7464867.47136</v>
       </c>
       <c r="N38" s="8">
-        <v>-116166.955008</v>
+        <v>-248828.915712</v>
       </c>
       <c r="O38" s="8">
         <v>8</v>
@@ -3795,10 +3937,10 @@
         <v>1</v>
       </c>
       <c r="Q38" s="8">
-        <v>508230.42816</v>
+        <v>0</v>
       </c>
       <c r="R38" s="8">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="S38" s="8">
         <v>0</v>
@@ -3810,18 +3952,18 @@
         <v>0</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X38" s="1">
-        <v>14290</v>
+        <v>14291</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="A39" s="7">
-        <v>43374</v>
+        <v>43344</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8">
@@ -3834,43 +3976,43 @@
         <v>25</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>29</v>
       </c>
       <c r="J39" s="8">
-        <v>3966012.44832</v>
+        <v>5474236.145664</v>
       </c>
       <c r="K39" s="8">
-        <v>2065440</v>
+        <v>4424160</v>
       </c>
       <c r="L39" s="8">
         <v>0.5</v>
       </c>
       <c r="M39" s="8">
-        <v>3485008.65024</v>
+        <v>7464867.47136</v>
       </c>
       <c r="N39" s="8">
-        <v>0</v>
+        <v>-1990631.325696</v>
       </c>
       <c r="O39" s="8">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="P39" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q39" s="8">
-        <v>481003.79808</v>
+        <v>0</v>
       </c>
       <c r="R39" s="8">
-        <v>26.5</v>
+        <v>0</v>
       </c>
       <c r="S39" s="8">
         <v>0</v>
@@ -3882,18 +4024,18 @@
         <v>0</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X39" s="1">
-        <v>14236</v>
+        <v>14290</v>
       </c>
     </row>
     <row r="40" spans="1:24">
       <c r="A40" s="7">
-        <v>43313</v>
+        <v>43374</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8">
@@ -3906,16 +4048,16 @@
         <v>25</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="J40" s="8">
         <v>7464867.47136</v>
@@ -3954,40 +4096,1192 @@
         <v>0</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="W40" s="1" t="s">
         <v>31</v>
       </c>
       <c r="X40" s="1">
+        <v>14236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24">
+      <c r="A41" s="7">
+        <v>43313</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J41" s="8">
+        <v>3797207.341824</v>
+      </c>
+      <c r="K41" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L41" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M41" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N41" s="8">
+        <v>-232333.910016</v>
+      </c>
+      <c r="O41" s="8">
+        <v>16</v>
+      </c>
+      <c r="P41" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q41" s="8">
+        <v>544532.6016</v>
+      </c>
+      <c r="R41" s="8">
+        <v>26.5</v>
+      </c>
+      <c r="S41" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="T41" s="8">
+        <v>0</v>
+      </c>
+      <c r="U41" s="8">
+        <v>0</v>
+      </c>
+      <c r="V41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X41" s="1">
         <v>14291</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41"/>
-      <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-      <c r="X41"/>
+    <row r="42" spans="1:24">
+      <c r="A42" s="7">
+        <v>43344</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="8">
+        <v>2758965.18144</v>
+      </c>
+      <c r="K42" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L42" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M42" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N42" s="8">
+        <v>-1161669.55008</v>
+      </c>
+      <c r="O42" s="8">
+        <v>80</v>
+      </c>
+      <c r="P42" s="8">
+        <v>10</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>435626.08128</v>
+      </c>
+      <c r="R42" s="8">
+        <v>24</v>
+      </c>
+      <c r="S42" s="8">
+        <v>0</v>
+      </c>
+      <c r="T42" s="8">
+        <v>0</v>
+      </c>
+      <c r="U42" s="8">
+        <v>0</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X42" s="1">
+        <v>14290</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24">
+      <c r="A43" s="7">
+        <v>43374</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J43" s="8">
+        <v>3748199.40768</v>
+      </c>
+      <c r="K43" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L43" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M43" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N43" s="8">
+        <v>0</v>
+      </c>
+      <c r="O43" s="8">
+        <v>0</v>
+      </c>
+      <c r="P43" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="8">
+        <v>263190.75744</v>
+      </c>
+      <c r="R43" s="8">
+        <v>14.5</v>
+      </c>
+      <c r="S43" s="8">
+        <v>0</v>
+      </c>
+      <c r="T43" s="8">
+        <v>0</v>
+      </c>
+      <c r="U43" s="8">
+        <v>0</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X43" s="1">
+        <v>14236</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24">
+      <c r="A44" s="7">
+        <v>43313</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J44" s="8">
+        <v>3602990.71392</v>
+      </c>
+      <c r="K44" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L44" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M44" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N44" s="8">
+        <v>0</v>
+      </c>
+      <c r="O44" s="8">
+        <v>0</v>
+      </c>
+      <c r="P44" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>117982.06368</v>
+      </c>
+      <c r="R44" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="S44" s="8">
+        <v>0</v>
+      </c>
+      <c r="T44" s="8">
+        <v>0</v>
+      </c>
+      <c r="U44" s="8">
+        <v>0</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X44" s="1">
+        <v>14291</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24">
+      <c r="A45" s="7">
+        <v>43344</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J45" s="8">
+        <v>2555673.010176</v>
+      </c>
+      <c r="K45" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L45" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M45" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N45" s="8">
+        <v>-929335.640064</v>
+      </c>
+      <c r="O45" s="8">
+        <v>64</v>
+      </c>
+      <c r="P45" s="8">
+        <v>8</v>
+      </c>
+      <c r="Q45" s="8">
+        <v>0</v>
+      </c>
+      <c r="R45" s="8">
+        <v>0</v>
+      </c>
+      <c r="S45" s="8">
+        <v>0</v>
+      </c>
+      <c r="T45" s="8">
+        <v>0</v>
+      </c>
+      <c r="U45" s="8">
+        <v>0</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X45" s="1">
+        <v>14290</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24">
+      <c r="A46" s="7">
+        <v>43313</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J46" s="8">
+        <v>3639292.88736</v>
+      </c>
+      <c r="K46" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L46" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M46" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N46" s="8">
+        <v>0</v>
+      </c>
+      <c r="O46" s="8">
+        <v>0</v>
+      </c>
+      <c r="P46" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>154284.23712</v>
+      </c>
+      <c r="R46" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="S46" s="8">
+        <v>0</v>
+      </c>
+      <c r="T46" s="8">
+        <v>0</v>
+      </c>
+      <c r="U46" s="8">
+        <v>0</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X46" s="1">
+        <v>14291</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24">
+      <c r="A47" s="7">
+        <v>43344</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" s="8">
+        <v>3584839.6272</v>
+      </c>
+      <c r="K47" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L47" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M47" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N47" s="8">
+        <v>0</v>
+      </c>
+      <c r="O47" s="8">
+        <v>0</v>
+      </c>
+      <c r="P47" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="8">
+        <v>99830.97696</v>
+      </c>
+      <c r="R47" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="S47" s="8">
+        <v>0</v>
+      </c>
+      <c r="T47" s="8">
+        <v>0</v>
+      </c>
+      <c r="U47" s="8">
+        <v>0</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="W47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X47" s="1">
+        <v>14290</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24">
+      <c r="A48" s="7">
+        <v>43374</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" s="8">
+        <v>3593915.17056</v>
+      </c>
+      <c r="K48" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L48" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M48" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N48" s="8">
+        <v>0</v>
+      </c>
+      <c r="O48" s="8">
+        <v>0</v>
+      </c>
+      <c r="P48" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="8">
+        <v>108906.52032</v>
+      </c>
+      <c r="R48" s="8">
+        <v>6</v>
+      </c>
+      <c r="S48" s="8">
+        <v>0</v>
+      </c>
+      <c r="T48" s="8">
+        <v>0</v>
+      </c>
+      <c r="U48" s="8">
+        <v>0</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="W48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X48" s="1">
+        <v>14236</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24">
+      <c r="A49" s="7">
+        <v>43313</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J49" s="8">
+        <v>3759090.059712</v>
+      </c>
+      <c r="K49" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L49" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M49" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N49" s="8">
+        <v>-116166.955008</v>
+      </c>
+      <c r="O49" s="8">
+        <v>8</v>
+      </c>
+      <c r="P49" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>390248.36448</v>
+      </c>
+      <c r="R49" s="8">
+        <v>21.5</v>
+      </c>
+      <c r="S49" s="8">
+        <v>0</v>
+      </c>
+      <c r="T49" s="8">
+        <v>0</v>
+      </c>
+      <c r="U49" s="8">
+        <v>0</v>
+      </c>
+      <c r="V49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="W49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X49" s="1">
+        <v>14291</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
+      <c r="A50" s="7">
+        <v>43344</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J50" s="8">
+        <v>3877072.123392</v>
+      </c>
+      <c r="K50" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L50" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M50" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N50" s="8">
+        <v>-116166.955008</v>
+      </c>
+      <c r="O50" s="8">
+        <v>8</v>
+      </c>
+      <c r="P50" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>508230.42816</v>
+      </c>
+      <c r="R50" s="8">
+        <v>28</v>
+      </c>
+      <c r="S50" s="8">
+        <v>0</v>
+      </c>
+      <c r="T50" s="8">
+        <v>0</v>
+      </c>
+      <c r="U50" s="8">
+        <v>0</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X50" s="1">
+        <v>14290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24">
+      <c r="A51" s="7">
+        <v>43374</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J51" s="8">
+        <v>3966012.44832</v>
+      </c>
+      <c r="K51" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L51" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M51" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N51" s="8">
+        <v>0</v>
+      </c>
+      <c r="O51" s="8">
+        <v>0</v>
+      </c>
+      <c r="P51" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="8">
+        <v>481003.79808</v>
+      </c>
+      <c r="R51" s="8">
+        <v>26.5</v>
+      </c>
+      <c r="S51" s="8">
+        <v>0</v>
+      </c>
+      <c r="T51" s="8">
+        <v>0</v>
+      </c>
+      <c r="U51" s="8">
+        <v>0</v>
+      </c>
+      <c r="V51" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X51" s="1">
+        <v>14236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24">
+      <c r="A52" s="7">
+        <v>43313</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J52" s="8">
+        <v>3252674.740224</v>
+      </c>
+      <c r="K52" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L52" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M52" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N52" s="8">
+        <v>-232333.910016</v>
+      </c>
+      <c r="O52" s="8">
+        <v>16</v>
+      </c>
+      <c r="P52" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q52" s="8">
+        <v>0</v>
+      </c>
+      <c r="R52" s="8">
+        <v>0</v>
+      </c>
+      <c r="S52" s="8">
+        <v>0</v>
+      </c>
+      <c r="T52" s="8">
+        <v>0</v>
+      </c>
+      <c r="U52" s="8">
+        <v>0</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X52" s="1">
+        <v>14291</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24">
+      <c r="A53" s="7">
+        <v>43344</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J53" s="8">
+        <v>3368841.695232</v>
+      </c>
+      <c r="K53" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L53" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M53" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N53" s="8">
+        <v>-116166.955008</v>
+      </c>
+      <c r="O53" s="8">
+        <v>8</v>
+      </c>
+      <c r="P53" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>0</v>
+      </c>
+      <c r="R53" s="8">
+        <v>0</v>
+      </c>
+      <c r="S53" s="8">
+        <v>0</v>
+      </c>
+      <c r="T53" s="8">
+        <v>0</v>
+      </c>
+      <c r="U53" s="8">
+        <v>0</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="W53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X53" s="1">
+        <v>14290</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24">
+      <c r="A54" s="7">
+        <v>43374</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J54" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="K54" s="8">
+        <v>2065440</v>
+      </c>
+      <c r="L54" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M54" s="8">
+        <v>3485008.65024</v>
+      </c>
+      <c r="N54" s="8">
+        <v>0</v>
+      </c>
+      <c r="O54" s="8">
+        <v>0</v>
+      </c>
+      <c r="P54" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="8">
+        <v>0</v>
+      </c>
+      <c r="R54" s="8">
+        <v>0</v>
+      </c>
+      <c r="S54" s="8">
+        <v>0</v>
+      </c>
+      <c r="T54" s="8">
+        <v>0</v>
+      </c>
+      <c r="U54" s="8">
+        <v>0</v>
+      </c>
+      <c r="V54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X54" s="1">
+        <v>14236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24">
+      <c r="A55" s="7">
+        <v>43374</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J55" s="8">
+        <v>6967209.09829149</v>
+      </c>
+      <c r="K55" s="8">
+        <v>4424159.6152</v>
+      </c>
+      <c r="L55" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M55" s="8">
+        <v>7464866.88643072</v>
+      </c>
+      <c r="N55" s="8">
+        <v>-497657.788139233</v>
+      </c>
+      <c r="O55" s="8">
+        <v>16</v>
+      </c>
+      <c r="P55" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q55" s="8">
+        <v>0</v>
+      </c>
+      <c r="R55" s="8">
+        <v>0</v>
+      </c>
+      <c r="S55" s="8">
+        <v>0</v>
+      </c>
+      <c r="T55" s="8">
+        <v>0</v>
+      </c>
+      <c r="U55" s="8">
+        <v>0</v>
+      </c>
+      <c r="V55" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="W55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X55" s="1">
+        <v>14236</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24">
+      <c r="A56" s="7">
+        <v>43313</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8">
+        <v>1577</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J56" s="8">
+        <v>7464867.47136</v>
+      </c>
+      <c r="K56" s="8">
+        <v>4424160</v>
+      </c>
+      <c r="L56" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M56" s="8">
+        <v>7464867.47136</v>
+      </c>
+      <c r="N56" s="8">
+        <v>0</v>
+      </c>
+      <c r="O56" s="8">
+        <v>0</v>
+      </c>
+      <c r="P56" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="8">
+        <v>0</v>
+      </c>
+      <c r="R56" s="8">
+        <v>0</v>
+      </c>
+      <c r="S56" s="8">
+        <v>0</v>
+      </c>
+      <c r="T56" s="8">
+        <v>0</v>
+      </c>
+      <c r="U56" s="8">
+        <v>0</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X56" s="1">
+        <v>14291</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+      <c r="S57"/>
+      <c r="T57"/>
+      <c r="U57"/>
+      <c r="V57"/>
+      <c r="W57"/>
+      <c r="X57"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>